<commit_message>
21 - 10 - 2021
</commit_message>
<xml_diff>
--- a/Chandan_Shalab_TestNG_Data_Driven_Framework/src/main/java/Data_Source/User_Data.xlsx
+++ b/Chandan_Shalab_TestNG_Data_Driven_Framework/src/main/java/Data_Source/User_Data.xlsx
@@ -143,7 +143,7 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D13" activeCellId="0" sqref="D13"/>
+      <selection pane="topLeft" activeCell="E11" activeCellId="0" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -205,7 +205,7 @@
       <selection pane="topLeft" activeCell="C19" activeCellId="0" sqref="C19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>